<commit_message>
test: gas biasing circuit
</commit_message>
<xml_diff>
--- a/hardware/gas_nrf52832/pcb/3차_Rev1.0.3/SMT/bom.xlsx
+++ b/hardware/gas_nrf52832/pcb/3차_Rev1.0.3/SMT/bom.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradkim06/hhs/docker/work/gas_ces/hardware/gas_nrf52832/pcb/SMT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradkim06/hhs/docker/work/gas_ces/hardware/gas_nrf52832/pcb/3차_Rev1.0.3/SMT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B0B35E73-0416-B94D-9602-BCDBB008E525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DD99467E-69C8-E846-B545-0E3FDC411DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="500" windowWidth="47980" windowHeight="28300" xr2:uid="{2507D3DE-0913-D943-A126-F509073BA56B}"/>
+    <workbookView xWindow="56080" yWindow="500" windowWidth="41440" windowHeight="28300" xr2:uid="{2507D3DE-0913-D943-A126-F509073BA56B}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="215" uniqueCount="146">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="220" uniqueCount="151">
   <si>
     <t>Reference</t>
   </si>
@@ -463,6 +474,26 @@
   </si>
   <si>
     <t>SMD3215-2P</t>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1차</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3차</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1055,8 +1086,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1434,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3E1E96-E31F-1543-A0AF-E6EF5F44CD5D}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1449,7 +1486,7 @@
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1474,60 +1511,113 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="I1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J2" s="1">
+        <f>20*C2</f>
+        <v>40</v>
+      </c>
+      <c r="K2" s="1">
+        <f>20*C2</f>
+        <v>40</v>
+      </c>
+      <c r="L2" s="1">
+        <f>20*C2</f>
+        <v>40</v>
+      </c>
+      <c r="M2" s="1">
+        <f t="shared" ref="M2:M3" si="0">I2-J2-K2-L2</f>
+        <v>9880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="1">
+        <f>20*C3</f>
+        <v>120</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K31" si="1">20*C3</f>
+        <v>120</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L31" si="2">20*C3</f>
+        <v>120</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1552,8 +1642,27 @@
       <c r="H4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>10000</v>
+      </c>
+      <c r="J4">
+        <f>20*C4</f>
+        <v>80</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="M4">
+        <f>I4-J4-K4-L4</f>
+        <v>9760</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1578,372 +1687,652 @@
       <c r="H5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="I5">
+        <v>10000</v>
+      </c>
+      <c r="J5">
+        <f>20*C5</f>
+        <v>160</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M31" si="3">I5-J5-K5-L5</f>
+        <v>9520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J6">
+        <f>20*C6</f>
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>4940</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="1" customFormat="1">
+      <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1">
+        <v>500</v>
+      </c>
+      <c r="J7" s="1">
+        <f>20*C7</f>
+        <v>20</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="1">
+        <v>500</v>
+      </c>
+      <c r="J8" s="1">
+        <f>20*C8</f>
+        <v>20</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="1">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1">
+        <f>20*C9</f>
+        <v>20</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1">
+      <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1">
+        <v>500</v>
+      </c>
+      <c r="J10" s="1">
+        <f>20*C10</f>
+        <v>40</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="3"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="2">
+        <v>200</v>
+      </c>
+      <c r="J11" s="2">
+        <f>20*C11</f>
+        <v>60</v>
+      </c>
+      <c r="K11" s="2">
+        <v>84</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
+      <c r="H12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="1">
+        <v>100</v>
+      </c>
+      <c r="J12" s="1">
+        <f>20*C12</f>
+        <v>20</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1">
+        <v>200</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1">
+      <c r="A14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
+      <c r="H14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="1">
+        <v>500</v>
+      </c>
+      <c r="J14" s="1">
+        <f>20*C14</f>
+        <v>20</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1">
+      <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="H15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="1">
+        <v>500</v>
+      </c>
+      <c r="J15" s="1">
+        <f>20*C15</f>
+        <v>20</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="H16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="1">
+        <v>500</v>
+      </c>
+      <c r="J16" s="1">
+        <f>20*C16</f>
+        <v>20</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1">
+      <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
+      <c r="H17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="1">
+        <v>500</v>
+      </c>
+      <c r="J17" s="1">
+        <f>20*C17</f>
+        <v>20</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="1" customFormat="1">
+      <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
+      <c r="H18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="1">
+        <v>500</v>
+      </c>
+      <c r="J18" s="1">
+        <f>20*C18</f>
+        <v>20</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="1" customFormat="1">
+      <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="H19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J19" s="1">
+        <f>20*C19</f>
+        <v>40</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="3"/>
+        <v>9880</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -1968,295 +2357,524 @@
       <c r="H20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
+      <c r="I20" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J20">
+        <f>20*C20</f>
+        <v>40</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>9880</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1">
+      <c r="A21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>3</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J21" s="1">
+        <f>20*C21</f>
+        <v>60</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="3"/>
+        <v>9820</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1">
+      <c r="A22" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J22" s="1">
+        <f>20*C22</f>
+        <v>20</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="3"/>
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="1" customFormat="1">
+      <c r="A23" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="H23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J23" s="1">
+        <f>20*C23</f>
+        <v>20</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="3"/>
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="1" customFormat="1">
+      <c r="A24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>100</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="H24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J24" s="1">
+        <f>20*C24</f>
+        <v>20</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="3"/>
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="1" customFormat="1">
+      <c r="A25" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
+      <c r="H25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J25" s="1">
+        <f>20*C25</f>
+        <v>20</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="3"/>
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1">
+      <c r="A26" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>10</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
+      <c r="H26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J26" s="1">
+        <f>20*C26</f>
+        <v>60</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="3"/>
+        <v>9820</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="1" customFormat="1">
+      <c r="A27" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
+      <c r="H27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J27" s="1">
+        <f>20*C27</f>
+        <v>20</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="3"/>
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1">
+      <c r="A28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>150</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
+      <c r="H28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J28" s="1">
+        <f>20*C28</f>
+        <v>20</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="3"/>
+        <v>9940</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1">
+      <c r="A29" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>2</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
+      <c r="H29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J29" s="1">
+        <f>20*C29</f>
+        <v>40</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="3"/>
+        <v>9880</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1">
+      <c r="A30" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
+      <c r="H30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="1">
+        <v>100</v>
+      </c>
+      <c r="J30" s="1">
+        <f>20*C30</f>
+        <v>20</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1">
+      <c r="A31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H31" t="s">
-        <v>14</v>
+      <c r="H31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="1">
+        <v>200</v>
+      </c>
+      <c r="J31" s="1">
+        <f>20*C31</f>
+        <v>20</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="3"/>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>